<commit_message>
added test cases and utils
</commit_message>
<xml_diff>
--- a/src/test/resources/Hotstar_Data.xlsx
+++ b/src/test/resources/Hotstar_Data.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pavitmut\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pavitmut\IdeaProjects\Cucumber\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8FA1796-35CC-4114-8CA8-26932AABFCB9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB87C881-6592-46BF-AB4A-2ED41EC15710}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{319A5F86-A61E-4931-BC21-EB2BF05A2482}"/>
   </bookViews>
@@ -47,7 +47,7 @@
     <t>TypeValue</t>
   </si>
   <si>
-    <t>'movies'</t>
+    <t>movies</t>
   </si>
 </sst>
 </file>
@@ -92,12 +92,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -414,15 +417,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E6C8039D-D768-4822-A82B-3F8ECC8A0DFB}">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD2"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="43.6328125" customWidth="1"/>
+    <col min="1" max="1" width="52.54296875" customWidth="1"/>
+    <col min="3" max="3" width="11.90625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
@@ -441,6 +445,10 @@
         <v>3</v>
       </c>
     </row>
+    <row r="3" spans="1:2">
+      <c r="A3" s="1"/>
+      <c r="B3" s="3"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
Modified files are added
</commit_message>
<xml_diff>
--- a/src/test/resources/Hotstar_Data.xlsx
+++ b/src/test/resources/Hotstar_Data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pavitmut\IdeaProjects\Cucumber\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB87C881-6592-46BF-AB4A-2ED41EC15710}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77D9C6F9-D3D7-4C5E-9D96-7103A70BA192}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{319A5F86-A61E-4931-BC21-EB2BF05A2482}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>Verify that the user can able to search a movies</t>
   </si>
@@ -48,6 +48,12 @@
   </si>
   <si>
     <t>movies</t>
+  </si>
+  <si>
+    <t>verify that user able to access the kids successfully.</t>
+  </si>
+  <si>
+    <t>princess</t>
   </si>
 </sst>
 </file>
@@ -92,7 +98,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -102,6 +108,9 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -417,15 +426,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E6C8039D-D768-4822-A82B-3F8ECC8A0DFB}">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
     <col min="1" max="1" width="52.54296875" customWidth="1"/>
+    <col min="2" max="2" width="26.90625" customWidth="1"/>
     <col min="3" max="3" width="11.90625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -446,8 +456,16 @@
       </c>
     </row>
     <row r="3" spans="1:2">
-      <c r="A3" s="1"/>
-      <c r="B3" s="3"/>
+      <c r="A3" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" s="1"/>
+      <c r="B4" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>